<commit_message>
added json iteration coding
</commit_message>
<xml_diff>
--- a/src/main/resources/mapper.xlsx
+++ b/src/main/resources/mapper.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmodhugu\Desktop\Innovation_code_generator\code-generator\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\addade\git\codegenerator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCFD0EA9-0E3F-4918-9AAA-043E3086F149}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DBB645FD-6A8D-4419-BEC6-EA266A56BBCB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210" xr2:uid="{FF58773B-27F5-4D52-B688-F752179FA984}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Business Field</t>
   </si>
@@ -45,16 +45,52 @@
     <t>(Claim) IPAR Transmission Rule</t>
   </si>
   <si>
-    <t>InsuranceClaim.Mediclaim.Claimheader.claimType</t>
-  </si>
-  <si>
-    <t>InsuranceClaim.Mediclaim.Claimheader.corporateEntityCode</t>
-  </si>
-  <si>
-    <t>InsuranceClaim.Mediclaim.Claimheader.iparTransmissionRule</t>
-  </si>
-  <si>
-    <t>InsuranceClaim.Mediclaim.Claimheader.discountType</t>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.claimType</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.iparTransmissionRule</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.discountType</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.corporateEntityCode</t>
+  </si>
+  <si>
+    <t>(Claim) Total Allowed Amount</t>
+  </si>
+  <si>
+    <t>(Claim) Ineligible Amount</t>
+  </si>
+  <si>
+    <t>(Claim) Total Billed Amount</t>
+  </si>
+  <si>
+    <t>(Claim) Eligible Amount</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.totalAllowedAmount</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.ineligibleAmount</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.totalBilledAmount</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.eligibleAmount</t>
+  </si>
+  <si>
+    <t>(Claim) Ineligible Reason Code</t>
+  </si>
+  <si>
+    <t>(Claim) State</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.ineligibleReasonCode</t>
+  </si>
+  <si>
+    <t>InsuranceClaim.Mediclaim.ClaimHeader.state</t>
   </si>
 </sst>
 </file>
@@ -415,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6423E8B-8E97-4611-8190-5AE344A36495}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -448,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -456,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -464,7 +500,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>